<commit_message>
Teste carregar dados cliente OK
</commit_message>
<xml_diff>
--- a/data/base_clientes_excel.xlsx
+++ b/data/base_clientes_excel.xlsx
@@ -144,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +155,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -188,29 +194,29 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -542,7 +548,7 @@
     <col min="11" max="11" style="9" width="10.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>45468</v>
       </c>
@@ -612,7 +618,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>45468</v>
       </c>
@@ -647,7 +653,7 @@
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>45468</v>
       </c>
@@ -682,7 +688,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>45468</v>
       </c>
@@ -717,7 +723,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>45468</v>
       </c>
@@ -752,7 +758,7 @@
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>45468</v>
       </c>
@@ -787,7 +793,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>45468</v>
       </c>
@@ -822,7 +828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>45468</v>
       </c>
@@ -857,7 +863,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>45468</v>
       </c>
@@ -892,7 +898,7 @@
         <v>138</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>45468</v>
       </c>
@@ -927,7 +933,7 @@
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>45468</v>
       </c>
@@ -962,7 +968,7 @@
         <v>127</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>45468</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>45468</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>136</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>45468</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>45468</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>45468</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>45468</v>
       </c>
@@ -1172,7 +1178,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>45468</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>45468</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>45468</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4">
         <v>45468</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4">
         <v>45468</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>45468</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>45468</v>
       </c>
@@ -1417,7 +1423,7 @@
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4">
         <v>45468</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4">
         <v>45468</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4">
         <v>45468</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4">
         <v>45468</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4">
         <v>45468</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="4">
         <v>45468</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="4">
         <v>45468</v>
       </c>
@@ -1662,7 +1668,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="4">
         <v>45468</v>
       </c>
@@ -1697,7 +1703,7 @@
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="4">
         <v>45468</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>150</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="4">
         <v>45468</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="4">
         <v>45468</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="4">
         <v>45468</v>
       </c>

</xml_diff>

<commit_message>
Correção bug botão novo chat
</commit_message>
<xml_diff>
--- a/data/base_clientes_excel.xlsx
+++ b/data/base_clientes_excel.xlsx
@@ -1828,7 +1828,7 @@
         <v>126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1">
         <v>45468</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1">
         <v>45468</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1">
         <v>45468</v>
       </c>

</xml_diff>

<commit_message>
Subindo versão alpha do Sander
</commit_message>
<xml_diff>
--- a/data/base_clientes_excel.xlsx
+++ b/data/base_clientes_excel.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe570407d8e87ac/Área de Trabalho/Data Science/Gen AI/projetos/chatbot-whatsapp/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_BCB8FF268EC24EE56AE611CAF1AFA70A92500538" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF70A360-F408-4517-AC42-537AEAB449DB}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -142,8 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,40 +192,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -231,10 +239,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -272,71 +280,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -364,7 +372,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -387,11 +395,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -400,13 +408,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -416,7 +424,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -425,7 +433,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -434,7 +442,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -442,10 +450,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -510,3523 +518,3523 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45468</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
         <v>34366343878</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="1">
         <v>35800</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="7">
         <v>831783229</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="5">
         <v>3722.86</v>
       </c>
       <c r="K2" s="2">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45468</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="7">
         <v>72388905850</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="1">
         <v>28046</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="7">
         <v>314939234</v>
       </c>
-      <c r="J3" s="4">
-        <v>4745.23</v>
+      <c r="J3" s="5">
+        <v>4745.2299999999996</v>
       </c>
       <c r="K3" s="2">
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45468</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>85044167398</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>29167</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="7">
         <v>216507078</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="5">
         <v>6468.61</v>
       </c>
       <c r="K4" s="2">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45468</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="7">
         <v>86406862031</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1">
         <v>31842</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="7">
         <v>951937536</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>8144.83</v>
       </c>
       <c r="K5" s="2">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45468</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>84634445204</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="1">
         <v>24435</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="7">
         <v>968254040</v>
       </c>
-      <c r="J6" s="4">
-        <v>8466.54</v>
+      <c r="J6" s="5">
+        <v>8466.5400000000009</v>
       </c>
       <c r="K6" s="2">
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45468</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>43467189571</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="1">
         <v>23868</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="7">
         <v>576241830</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="5">
         <v>9934.66</v>
       </c>
       <c r="K7" s="2">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45468</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="7">
         <v>21573531600</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="1">
         <v>37807</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="7">
         <v>206547227</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="5">
         <v>7768.27</v>
       </c>
       <c r="K8" s="2">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45468</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="7">
         <v>96285056706</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="1">
         <v>33351</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="7">
         <v>831560063</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="5">
         <v>7369.88</v>
       </c>
       <c r="K9" s="2">
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45468</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>91103415018</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="1">
         <v>36105</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="7">
         <v>443851264</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="5">
         <v>3127.08</v>
       </c>
       <c r="K10" s="2">
         <v>138</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45468</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="7">
         <v>32985101735</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="1">
         <v>35700</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="7">
         <v>551118298</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="5">
         <v>2522.56</v>
       </c>
       <c r="K11" s="2">
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45468</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="7">
         <v>15070784471</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
         <v>32</v>
       </c>
       <c r="G12" s="1">
         <v>30776</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="7">
         <v>122414616</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="5">
         <v>1207.3</v>
       </c>
       <c r="K12" s="2">
         <v>127</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45468</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="7">
         <v>48401648270</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="1">
         <v>35254</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="7">
         <v>148104050</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="5">
         <v>7039.15</v>
       </c>
       <c r="K13" s="2">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45468</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="7">
         <v>30948448040</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="1">
         <v>25270</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="7">
         <v>981282343</v>
       </c>
-      <c r="J14" s="4">
-        <v>9831.46</v>
+      <c r="J14" s="5">
+        <v>9831.4599999999991</v>
       </c>
       <c r="K14" s="2">
         <v>136</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45468</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="7">
         <v>2343959668</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="1">
         <v>32006</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="7">
         <v>620838110</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="5">
         <v>5755.52</v>
       </c>
       <c r="K15" s="2">
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45468</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="7">
         <v>12697030646</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1">
         <v>23700</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="7">
         <v>122753875</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="5">
         <v>7078.09</v>
       </c>
       <c r="K16" s="2">
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45468</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="7">
         <v>62869488050</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="1">
         <v>24461</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="7">
         <v>619360421</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="5">
         <v>1629.36</v>
       </c>
       <c r="K17" s="2">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45468</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="7">
         <v>39053994238</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="1">
         <v>24957</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="7">
         <v>862813598</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="5">
         <v>6551.07</v>
       </c>
       <c r="K18" s="2">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45468</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="7">
         <v>59333293477</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="1">
         <v>30495</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="7">
         <v>961081424</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="5">
         <v>5130.75</v>
       </c>
       <c r="K19" s="2">
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45468</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="7">
         <v>50856433306</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="1">
         <v>36834</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="7">
         <v>932387400</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="5">
         <v>8810.64</v>
       </c>
       <c r="K20" s="2">
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45468</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="7">
         <v>62824603879</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
         <v>19</v>
       </c>
       <c r="G21" s="1">
         <v>30030</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="7">
         <v>354995081</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="5">
         <v>8971.19</v>
       </c>
       <c r="K21" s="2">
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45468</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="7">
         <v>45160842446</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="1">
         <v>36102</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="7">
         <v>130441425</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="5">
         <v>6818.53</v>
       </c>
       <c r="K22" s="2">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45468</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="7">
         <v>47106320650</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
         <v>32</v>
       </c>
       <c r="G23" s="1">
         <v>37737</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="7">
         <v>833462015</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="5">
         <v>5518.69</v>
       </c>
       <c r="K23" s="2">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45468</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="7">
         <v>17069182597</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="1">
         <v>24425</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="7">
         <v>621064027</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="5">
         <v>4169.12</v>
       </c>
       <c r="K24" s="2">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45468</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="7">
         <v>9903213204</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="1">
         <v>29110</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="7">
         <v>666831812</v>
       </c>
-      <c r="J25" s="4">
-        <v>8330.22</v>
+      <c r="J25" s="5">
+        <v>8330.2199999999993</v>
       </c>
       <c r="K25" s="2">
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45468</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="7">
         <v>8932740380</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
         <v>32</v>
       </c>
       <c r="G26" s="1">
         <v>27048</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="7">
         <v>925664168</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="5">
         <v>6598.87</v>
       </c>
       <c r="K26" s="2">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45468</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="7">
         <v>19130508584</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="1">
         <v>28464</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="7">
         <v>334361699</v>
       </c>
-      <c r="J27" s="4">
-        <v>8591.72</v>
+      <c r="J27" s="5">
+        <v>8591.7199999999993</v>
       </c>
       <c r="K27" s="2">
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45468</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="7">
         <v>37352802266</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
         <v>32</v>
       </c>
       <c r="G28" s="1">
         <v>26840</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="7">
         <v>255137084</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="5">
         <v>6223.2</v>
       </c>
       <c r="K28" s="2">
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45468</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="7">
         <v>65360922605</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="1">
         <v>34224</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="7">
         <v>361145063</v>
       </c>
-      <c r="J29" s="4">
-        <v>9206.55</v>
+      <c r="J29" s="5">
+        <v>9206.5499999999993</v>
       </c>
       <c r="K29" s="2">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45468</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="7">
         <v>54832489704</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
         <v>19</v>
       </c>
       <c r="G30" s="1">
         <v>34896</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="7">
         <v>469266241</v>
       </c>
-      <c r="J30" s="4">
-        <v>9958.63</v>
+      <c r="J30" s="5">
+        <v>9958.6299999999992</v>
       </c>
       <c r="K30" s="2">
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45468</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="7">
         <v>31472259920</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="1">
         <v>36126</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="7">
         <v>835020757</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="5">
         <v>1212.98</v>
       </c>
       <c r="K31" s="2">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45468</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="7">
         <v>26095861241</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
         <v>32</v>
       </c>
       <c r="G32" s="1">
         <v>33212</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" t="s">
         <v>24</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="7">
         <v>525284308</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="5">
         <v>6458.39</v>
       </c>
       <c r="K32" s="2">
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45468</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="7">
         <v>70508473802</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
         <v>32</v>
       </c>
       <c r="G33" s="1">
         <v>36315</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="7">
         <v>537758087</v>
       </c>
-      <c r="J33" s="4">
-        <v>4536.02</v>
+      <c r="J33" s="5">
+        <v>4536.0200000000004</v>
       </c>
       <c r="K33" s="2">
         <v>132</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45468</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="7">
         <v>96743776386</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="1">
         <v>26976</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="7">
         <v>648419215</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="5">
         <v>8951.77</v>
       </c>
       <c r="K34" s="2">
         <v>150</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45468</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="7">
         <v>20081556845</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
         <v>32</v>
       </c>
       <c r="G35" s="1">
         <v>30673</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" t="s">
         <v>15</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="7">
         <v>965164213</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="5">
         <v>5666.3</v>
       </c>
       <c r="K35" s="2">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45468</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="7">
         <v>41827978252</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="3" t="s">
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
         <v>32</v>
       </c>
       <c r="G36" s="1">
         <v>33543</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="7">
         <v>565871051</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="5">
         <v>6802.26</v>
       </c>
       <c r="K36" s="2">
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45468</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="7">
         <v>18757138087</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
         <v>32</v>
       </c>
       <c r="G37" s="1">
         <v>32861</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="7">
         <v>253452842</v>
       </c>
-      <c r="J37" s="4">
-        <v>9044.05</v>
+      <c r="J37" s="5">
+        <v>9044.0499999999993</v>
       </c>
       <c r="K37" s="2">
         <v>126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45468</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="7">
         <v>19832949777</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="3" t="s">
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="1">
         <v>27096</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="7">
         <v>884016144</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="5">
         <v>3477.97</v>
       </c>
       <c r="K38" s="2">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45468</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="7">
         <v>12710946149</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="1">
         <v>28664</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="7">
         <v>440853979</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="5">
         <v>4072.14</v>
       </c>
       <c r="K39" s="2">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45468</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="7">
         <v>36513817145</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
         <v>32</v>
       </c>
       <c r="G40" s="1">
         <v>37430</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" t="s">
         <v>24</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="7">
         <v>894806104</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="5">
         <v>6244.47</v>
       </c>
       <c r="K40" s="2">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45468</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="7">
         <v>2354091621</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="3" t="s">
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
         <v>32</v>
       </c>
       <c r="G41" s="1">
         <v>36853</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="7">
         <v>434800250</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="5">
         <v>5489.85</v>
       </c>
       <c r="K41" s="2">
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45468</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="7">
         <v>13871071358</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="3" t="s">
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
         <v>19</v>
       </c>
       <c r="G42" s="1">
         <v>32746</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="7">
         <v>824345442</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="5">
         <v>5355.03</v>
       </c>
       <c r="K42" s="2">
         <v>144</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45468</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="7">
         <v>567017990</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="3" t="s">
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1">
         <v>28397</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" t="s">
         <v>22</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="7">
         <v>140587443</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="5">
         <v>4304.72</v>
       </c>
       <c r="K43" s="2">
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45468</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="7">
         <v>74914376210</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="3" t="s">
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
         <v>14</v>
       </c>
       <c r="G44" s="1">
         <v>25298</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="7">
         <v>141799424</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="5">
         <v>3030.77</v>
       </c>
       <c r="K44" s="2">
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45468</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="7">
         <v>92417518783</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="3" t="s">
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" t="s">
         <v>19</v>
       </c>
       <c r="G45" s="1">
         <v>26054</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" t="s">
         <v>15</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="7">
         <v>753518334</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="5">
         <v>4378.62</v>
       </c>
       <c r="K45" s="2">
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45468</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="7">
         <v>83353912037</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="1">
         <v>34526</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="7">
         <v>696759879</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="5">
         <v>2842.01</v>
       </c>
       <c r="K46" s="2">
         <v>144</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45468</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="7">
         <v>18320589053</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="3" t="s">
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="1">
         <v>30472</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" t="s">
         <v>24</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="7">
         <v>603462942</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="5">
         <v>1232.2</v>
       </c>
       <c r="K47" s="2">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45468</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="7">
         <v>15129585062</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="3" t="s">
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
         <v>32</v>
       </c>
       <c r="G48" s="1">
         <v>32749</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="7">
         <v>946055252</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48" s="5">
         <v>6033.06</v>
       </c>
       <c r="K48" s="2">
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45468</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="7">
         <v>14715451301</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="E49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="1">
         <v>35613</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="7">
         <v>143250499</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="5">
         <v>1560.67</v>
       </c>
       <c r="K49" s="2">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45468</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="7">
         <v>66989563257</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="3" t="s">
+      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="1">
         <v>37222</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="7">
         <v>843026029</v>
       </c>
-      <c r="J50" s="4">
-        <v>4649.9</v>
+      <c r="J50" s="5">
+        <v>4649.8999999999996</v>
       </c>
       <c r="K50" s="2">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>45468</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="7">
         <v>78553853985</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="3" t="s">
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="1">
         <v>27172</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="7">
         <v>949715742</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="5">
         <v>8245.74</v>
       </c>
       <c r="K51" s="2">
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>45468</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="7">
         <v>73778724037</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" t="s">
         <v>17</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="3" t="s">
+      <c r="E52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" t="s">
         <v>14</v>
       </c>
       <c r="G52" s="1">
         <v>32433</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="7">
         <v>211668543</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="5">
         <v>5971.56</v>
       </c>
       <c r="K52" s="2">
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>45468</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="7">
         <v>45865605330</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="3" t="s">
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
         <v>19</v>
       </c>
       <c r="G53" s="1">
         <v>36665</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" t="s">
         <v>22</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="7">
         <v>925355574</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="5">
         <v>5410.4</v>
       </c>
       <c r="K53" s="2">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>45468</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="7">
         <v>51295353911</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="3" t="s">
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s">
         <v>14</v>
       </c>
       <c r="G54" s="1">
         <v>27165</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" t="s">
         <v>24</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="7">
         <v>815136071</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54" s="5">
         <v>5571.13</v>
       </c>
       <c r="K54" s="2">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>45468</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="7">
         <v>97511848516</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="3" t="s">
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s">
         <v>32</v>
       </c>
       <c r="G55" s="1">
         <v>27629</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" t="s">
         <v>22</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="7">
         <v>636900930</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55" s="5">
         <v>3469.37</v>
       </c>
       <c r="K55" s="2">
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>45468</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="7">
         <v>86031984628</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
         <v>40</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" t="s">
         <v>17</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="3" t="s">
+      <c r="E56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="1">
         <v>27656</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="7">
         <v>626940829</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="5">
         <v>7520.03</v>
       </c>
       <c r="K56" s="2">
         <v>121</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>45468</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="7">
         <v>36254327490</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="3" t="s">
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
         <v>32</v>
       </c>
       <c r="G57" s="1">
         <v>27433</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H57" t="s">
         <v>24</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="7">
         <v>351472492</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="5">
         <v>659.61</v>
       </c>
       <c r="K57" s="2">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>45468</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="7">
         <v>60943415462</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" t="s">
         <v>34</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" t="s">
         <v>21</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="3" t="s">
+      <c r="E58" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" t="s">
         <v>14</v>
       </c>
       <c r="G58" s="1">
         <v>26230</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58" t="s">
         <v>24</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I58" s="7">
         <v>796920163</v>
       </c>
-      <c r="J58" s="4">
+      <c r="J58" s="5">
         <v>6501.17</v>
       </c>
       <c r="K58" s="2">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>45468</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="7">
         <v>68630599405</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="3" t="s">
+      <c r="E59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" t="s">
         <v>32</v>
       </c>
       <c r="G59" s="1">
         <v>30213</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H59" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I59" s="7">
         <v>444219392</v>
       </c>
-      <c r="J59" s="4">
+      <c r="J59" s="5">
         <v>6757.68</v>
       </c>
       <c r="K59" s="2">
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45468</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="7">
         <v>98840145826</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
         <v>38</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="3" t="s">
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" t="s">
         <v>32</v>
       </c>
       <c r="G60" s="1">
         <v>37779</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" t="s">
         <v>22</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I60" s="7">
         <v>796311028</v>
       </c>
-      <c r="J60" s="4">
+      <c r="J60" s="5">
         <v>6337.07</v>
       </c>
       <c r="K60" s="2">
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>45468</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="7">
         <v>55655611597</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="3" t="s">
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" t="s">
         <v>14</v>
       </c>
       <c r="G61" s="1">
         <v>25196</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" t="s">
         <v>24</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="7">
         <v>512661252</v>
       </c>
-      <c r="J61" s="4">
+      <c r="J61" s="5">
         <v>1627.09</v>
       </c>
       <c r="K61" s="2">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>45468</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="7">
         <v>47514943501</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="3" t="s">
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1">
         <v>24941</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" t="s">
         <v>24</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="7">
         <v>989765753</v>
       </c>
-      <c r="J62" s="4">
+      <c r="J62" s="5">
         <v>9893.52</v>
       </c>
       <c r="K62" s="2">
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45468</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="7">
         <v>31827850108</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" t="s">
         <v>38</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" s="3" t="s">
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
         <v>32</v>
       </c>
       <c r="G63" s="1">
         <v>34589</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H63" t="s">
         <v>15</v>
       </c>
-      <c r="I63" s="2">
+      <c r="I63" s="7">
         <v>963425881</v>
       </c>
-      <c r="J63" s="4">
+      <c r="J63" s="5">
         <v>6266.95</v>
       </c>
       <c r="K63" s="2">
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>45468</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="7">
         <v>35586995131</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" t="s">
         <v>36</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="3" t="s">
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" t="s">
         <v>32</v>
       </c>
       <c r="G64" s="1">
         <v>37430</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" t="s">
         <v>15</v>
       </c>
-      <c r="I64" s="2">
+      <c r="I64" s="7">
         <v>266290710</v>
       </c>
-      <c r="J64" s="4">
+      <c r="J64" s="5">
         <v>9339.24</v>
       </c>
       <c r="K64" s="2">
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>45468</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="7">
         <v>32887994212</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" t="s">
         <v>39</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" t="s">
         <v>32</v>
       </c>
       <c r="G65" s="1">
         <v>34047</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" t="s">
         <v>22</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I65" s="7">
         <v>190005720</v>
       </c>
-      <c r="J65" s="4">
+      <c r="J65" s="5">
         <v>7376.83</v>
       </c>
       <c r="K65" s="2">
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>45468</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="7">
         <v>81515128571</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" t="s">
         <v>21</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="3" t="s">
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
         <v>14</v>
       </c>
       <c r="G66" s="1">
         <v>28186</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="H66" t="s">
         <v>22</v>
       </c>
-      <c r="I66" s="2">
+      <c r="I66" s="7">
         <v>906026922</v>
       </c>
-      <c r="J66" s="4">
+      <c r="J66" s="5">
         <v>7960.17</v>
       </c>
       <c r="K66" s="2">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>45468</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="7">
         <v>46337510771</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" t="s">
         <v>34</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="3" t="s">
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" t="s">
         <v>14</v>
       </c>
       <c r="G67" s="1">
         <v>29485</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67" t="s">
         <v>15</v>
       </c>
-      <c r="I67" s="2">
+      <c r="I67" s="7">
         <v>698212548</v>
       </c>
-      <c r="J67" s="4">
+      <c r="J67" s="5">
         <v>6041.39</v>
       </c>
       <c r="K67" s="2">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>45468</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="7">
         <v>74950307983</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" t="s">
         <v>37</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="3" t="s">
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" t="s">
         <v>32</v>
       </c>
       <c r="G68" s="1">
         <v>28605</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" t="s">
         <v>24</v>
       </c>
-      <c r="I68" s="2">
+      <c r="I68" s="7">
         <v>343812440</v>
       </c>
-      <c r="J68" s="4">
+      <c r="J68" s="5">
         <v>502.4</v>
       </c>
       <c r="K68" s="2">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>45468</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="7">
         <v>99212293891</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" t="s">
         <v>21</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F69" s="3" t="s">
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" t="s">
         <v>14</v>
       </c>
       <c r="G69" s="1">
         <v>25641</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" t="s">
         <v>22</v>
       </c>
-      <c r="I69" s="2">
+      <c r="I69" s="7">
         <v>352747908</v>
       </c>
-      <c r="J69" s="4">
-        <v>5215.06</v>
+      <c r="J69" s="5">
+        <v>5215.0600000000004</v>
       </c>
       <c r="K69" s="2">
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>45468</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="7">
         <v>26031838850</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" t="s">
         <v>21</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="3" t="s">
+      <c r="E70" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" t="s">
         <v>19</v>
       </c>
       <c r="G70" s="1">
         <v>28903</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="H70" t="s">
         <v>24</v>
       </c>
-      <c r="I70" s="2">
+      <c r="I70" s="7">
         <v>489011092</v>
       </c>
-      <c r="J70" s="4">
-        <v>8329.21</v>
+      <c r="J70" s="5">
+        <v>8329.2099999999991</v>
       </c>
       <c r="K70" s="2">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row r="71" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>45468</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="7">
         <v>27215621693</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" t="s">
         <v>39</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="3" t="s">
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" t="s">
         <v>19</v>
       </c>
       <c r="G71" s="1">
         <v>29161</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="H71" t="s">
         <v>22</v>
       </c>
-      <c r="I71" s="2">
+      <c r="I71" s="7">
         <v>750851854</v>
       </c>
-      <c r="J71" s="4">
+      <c r="J71" s="5">
         <v>5115.29</v>
       </c>
       <c r="K71" s="2">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row r="72" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>45468</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="7">
         <v>48254478481</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" t="s">
         <v>21</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72" s="3" t="s">
+      <c r="E72" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" t="s">
         <v>32</v>
       </c>
       <c r="G72" s="1">
         <v>30176</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="H72" t="s">
         <v>24</v>
       </c>
-      <c r="I72" s="2">
+      <c r="I72" s="7">
         <v>586443030</v>
       </c>
-      <c r="J72" s="4">
-        <v>2068.7</v>
+      <c r="J72" s="5">
+        <v>2068.6999999999998</v>
       </c>
       <c r="K72" s="2">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row r="73" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>45468</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="7">
         <v>53108040219</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" t="s">
         <v>36</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" t="s">
         <v>17</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="3" t="s">
+      <c r="E73" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" t="s">
         <v>19</v>
       </c>
       <c r="G73" s="1">
         <v>24834</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="H73" t="s">
         <v>24</v>
       </c>
-      <c r="I73" s="2">
+      <c r="I73" s="7">
         <v>992346475</v>
       </c>
-      <c r="J73" s="4">
+      <c r="J73" s="5">
         <v>9007.51</v>
       </c>
       <c r="K73" s="2">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row r="74" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>45468</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="7">
         <v>36158596930</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" t="s">
         <v>39</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F74" s="3" t="s">
+      <c r="E74" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" t="s">
         <v>19</v>
       </c>
       <c r="G74" s="1">
         <v>25597</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H74" t="s">
         <v>24</v>
       </c>
-      <c r="I74" s="2">
+      <c r="I74" s="7">
         <v>949479640</v>
       </c>
-      <c r="J74" s="4">
+      <c r="J74" s="5">
         <v>3446.57</v>
       </c>
       <c r="K74" s="2">
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row r="75" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>45468</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="7">
         <v>86917178071</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="3" t="s">
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" t="s">
         <v>14</v>
       </c>
       <c r="G75" s="1">
         <v>33564</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H75" t="s">
         <v>22</v>
       </c>
-      <c r="I75" s="2">
+      <c r="I75" s="7">
         <v>422682571</v>
       </c>
-      <c r="J75" s="4">
+      <c r="J75" s="5">
         <v>4128.01</v>
       </c>
       <c r="K75" s="2">
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row r="76" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>45468</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="7">
         <v>2334281000</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" t="s">
         <v>30</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" t="s">
         <v>17</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F76" s="3" t="s">
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="1">
         <v>31578</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="H76" t="s">
         <v>24</v>
       </c>
-      <c r="I76" s="2">
+      <c r="I76" s="7">
         <v>199924796</v>
       </c>
-      <c r="J76" s="4">
+      <c r="J76" s="5">
         <v>1192.52</v>
       </c>
       <c r="K76" s="2">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>45468</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="7">
         <v>48180494330</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" t="s">
         <v>37</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="3" t="s">
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
         <v>19</v>
       </c>
       <c r="G77" s="1">
         <v>29802</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="H77" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="2">
+      <c r="I77" s="7">
         <v>548566190</v>
       </c>
-      <c r="J77" s="4">
+      <c r="J77" s="5">
         <v>5884.12</v>
       </c>
       <c r="K77" s="2">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>45468</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="7">
         <v>87607047050</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" t="s">
         <v>35</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" t="s">
         <v>21</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="3" t="s">
+      <c r="E78" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" t="s">
         <v>32</v>
       </c>
       <c r="G78" s="1">
         <v>34042</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="H78" t="s">
         <v>24</v>
       </c>
-      <c r="I78" s="2">
+      <c r="I78" s="7">
         <v>259429590</v>
       </c>
-      <c r="J78" s="4">
+      <c r="J78" s="5">
         <v>666.03</v>
       </c>
       <c r="K78" s="2">
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>45468</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="7">
         <v>9877822407</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" t="s">
         <v>36</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="3" t="s">
+      <c r="E79" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" t="s">
         <v>32</v>
       </c>
       <c r="G79" s="1">
         <v>27587</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="H79" t="s">
         <v>22</v>
       </c>
-      <c r="I79" s="2">
+      <c r="I79" s="7">
         <v>523898513</v>
       </c>
-      <c r="J79" s="4">
-        <v>8514.54</v>
+      <c r="J79" s="5">
+        <v>8514.5400000000009</v>
       </c>
       <c r="K79" s="2">
         <v>123</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row r="80" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45468</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="7">
         <v>46893244681</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" t="s">
         <v>36</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" t="s">
         <v>17</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" s="3" t="s">
+      <c r="E80" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" t="s">
         <v>32</v>
       </c>
       <c r="G80" s="1">
         <v>24906</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H80" t="s">
         <v>15</v>
       </c>
-      <c r="I80" s="2">
+      <c r="I80" s="7">
         <v>982953366</v>
       </c>
-      <c r="J80" s="4">
+      <c r="J80" s="5">
         <v>7564.3</v>
       </c>
       <c r="K80" s="2">
         <v>118</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row r="81" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>45468</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="7">
         <v>91496880650</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" t="s">
         <v>35</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="3" t="s">
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" t="s">
         <v>14</v>
       </c>
       <c r="G81" s="1">
         <v>28903</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="H81" t="s">
         <v>24</v>
       </c>
-      <c r="I81" s="2">
+      <c r="I81" s="7">
         <v>971767329</v>
       </c>
-      <c r="J81" s="4">
+      <c r="J81" s="5">
         <v>6198.71</v>
       </c>
       <c r="K81" s="2">
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row r="82" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>45468</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="7">
         <v>26311257548</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" t="s">
         <v>36</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="3" t="s">
+      <c r="E82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" t="s">
         <v>14</v>
       </c>
       <c r="G82" s="1">
         <v>28479</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" t="s">
         <v>15</v>
       </c>
-      <c r="I82" s="2">
+      <c r="I82" s="7">
         <v>216460524</v>
       </c>
-      <c r="J82" s="4">
+      <c r="J82" s="5">
         <v>5344.1</v>
       </c>
       <c r="K82" s="2">
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row r="83" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>45468</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="7">
         <v>99991639047</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F83" s="3" t="s">
+      <c r="E83" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" t="s">
         <v>14</v>
       </c>
       <c r="G83" s="1">
         <v>27361</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H83" t="s">
         <v>24</v>
       </c>
-      <c r="I83" s="2">
+      <c r="I83" s="7">
         <v>932710183</v>
       </c>
-      <c r="J83" s="4">
+      <c r="J83" s="5">
         <v>7482.94</v>
       </c>
       <c r="K83" s="2">
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row r="84" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>45468</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="7">
         <v>70599434120</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" t="s">
         <v>17</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="3" t="s">
+      <c r="E84" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" t="s">
         <v>32</v>
       </c>
       <c r="G84" s="1">
         <v>25515</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H84" t="s">
         <v>24</v>
       </c>
-      <c r="I84" s="2">
+      <c r="I84" s="7">
         <v>721333607</v>
       </c>
-      <c r="J84" s="4">
+      <c r="J84" s="5">
         <v>1338.03</v>
       </c>
       <c r="K84" s="2">
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row r="85" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>45468</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="7">
         <v>90986185612</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" t="s">
         <v>39</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" t="s">
         <v>17</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="3" t="s">
+      <c r="E85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" t="s">
         <v>19</v>
       </c>
       <c r="G85" s="1">
         <v>30044</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="H85" t="s">
         <v>15</v>
       </c>
-      <c r="I85" s="2">
+      <c r="I85" s="7">
         <v>214049208</v>
       </c>
-      <c r="J85" s="4">
+      <c r="J85" s="5">
         <v>9459.09</v>
       </c>
       <c r="K85" s="2">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row r="86" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>45468</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="7">
         <v>77515717645</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" t="s">
         <v>35</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" t="s">
         <v>17</v>
       </c>
-      <c r="E86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="3" t="s">
+      <c r="E86" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" t="s">
         <v>32</v>
       </c>
       <c r="G86" s="1">
         <v>23640</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="H86" t="s">
         <v>22</v>
       </c>
-      <c r="I86" s="2">
+      <c r="I86" s="7">
         <v>863592326</v>
       </c>
-      <c r="J86" s="4">
+      <c r="J86" s="5">
         <v>5850.43</v>
       </c>
       <c r="K86" s="2">
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row r="87" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>45468</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="7">
         <v>74608417576</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" t="s">
         <v>40</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F87" s="3" t="s">
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" t="s">
         <v>19</v>
       </c>
       <c r="G87" s="1">
         <v>36153</v>
       </c>
-      <c r="H87" s="3" t="s">
+      <c r="H87" t="s">
         <v>15</v>
       </c>
-      <c r="I87" s="2">
+      <c r="I87" s="7">
         <v>865659326</v>
       </c>
-      <c r="J87" s="4">
+      <c r="J87" s="5">
         <v>8411.24</v>
       </c>
       <c r="K87" s="2">
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row r="88" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>45468</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="7">
         <v>24071053380</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" t="s">
         <v>36</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F88" s="3" t="s">
+      <c r="E88" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" t="s">
         <v>19</v>
       </c>
       <c r="G88" s="1">
         <v>31316</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="H88" t="s">
         <v>15</v>
       </c>
-      <c r="I88" s="2">
+      <c r="I88" s="7">
         <v>825023534</v>
       </c>
-      <c r="J88" s="4">
-        <v>9097.29</v>
+      <c r="J88" s="5">
+        <v>9097.2900000000009</v>
       </c>
       <c r="K88" s="2">
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row r="89" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>45468</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="7">
         <v>88485580702</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" t="s">
         <v>33</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F89" s="3" t="s">
+      <c r="E89" t="s">
+        <v>18</v>
+      </c>
+      <c r="F89" t="s">
         <v>19</v>
       </c>
       <c r="G89" s="1">
         <v>25362</v>
       </c>
-      <c r="H89" s="3" t="s">
+      <c r="H89" t="s">
         <v>22</v>
       </c>
-      <c r="I89" s="2">
+      <c r="I89" s="7">
         <v>814920999</v>
       </c>
-      <c r="J89" s="4">
+      <c r="J89" s="5">
         <v>4464.28</v>
       </c>
       <c r="K89" s="2">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row r="90" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>45468</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="7">
         <v>62311319477</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" t="s">
         <v>38</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" t="s">
         <v>12</v>
       </c>
-      <c r="E90" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F90" s="3" t="s">
+      <c r="E90" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" t="s">
         <v>14</v>
       </c>
       <c r="G90" s="1">
         <v>25984</v>
       </c>
-      <c r="H90" s="3" t="s">
+      <c r="H90" t="s">
         <v>15</v>
       </c>
-      <c r="I90" s="2">
+      <c r="I90" s="7">
         <v>990069500</v>
       </c>
-      <c r="J90" s="4">
+      <c r="J90" s="5">
         <v>8274.94</v>
       </c>
       <c r="K90" s="2">
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row r="91" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>45468</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="7">
         <v>17949776005</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" t="s">
         <v>35</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="3" t="s">
+      <c r="E91" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" t="s">
         <v>14</v>
       </c>
       <c r="G91" s="1">
         <v>36163</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="H91" t="s">
         <v>22</v>
       </c>
-      <c r="I91" s="2">
+      <c r="I91" s="7">
         <v>316310947</v>
       </c>
-      <c r="J91" s="4">
+      <c r="J91" s="5">
         <v>2367.84</v>
       </c>
       <c r="K91" s="2">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row r="92" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>45468</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="7">
         <v>3509659279</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" t="s">
         <v>38</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" t="s">
         <v>17</v>
       </c>
-      <c r="E92" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92" s="3" t="s">
+      <c r="E92" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" t="s">
         <v>14</v>
       </c>
       <c r="G92" s="1">
         <v>28573</v>
       </c>
-      <c r="H92" s="3" t="s">
+      <c r="H92" t="s">
         <v>15</v>
       </c>
-      <c r="I92" s="2">
+      <c r="I92" s="7">
         <v>176855946</v>
       </c>
-      <c r="J92" s="4">
-        <v>8578.03</v>
+      <c r="J92" s="5">
+        <v>8578.0300000000007</v>
       </c>
       <c r="K92" s="2">
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row r="93" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>45468</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="7">
         <v>10320082610</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" t="s">
         <v>40</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" t="s">
         <v>17</v>
       </c>
-      <c r="E93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F93" s="3" t="s">
+      <c r="E93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" t="s">
         <v>14</v>
       </c>
       <c r="G93" s="1">
         <v>35209</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="H93" t="s">
         <v>22</v>
       </c>
-      <c r="I93" s="2">
+      <c r="I93" s="7">
         <v>674221680</v>
       </c>
-      <c r="J93" s="4">
+      <c r="J93" s="5">
         <v>5851.6</v>
       </c>
       <c r="K93" s="2">
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row r="94" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>45468</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="7">
         <v>51589942850</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" t="s">
         <v>36</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" t="s">
         <v>17</v>
       </c>
-      <c r="E94" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F94" s="3" t="s">
+      <c r="E94" t="s">
+        <v>18</v>
+      </c>
+      <c r="F94" t="s">
         <v>19</v>
       </c>
       <c r="G94" s="1">
         <v>33034</v>
       </c>
-      <c r="H94" s="3" t="s">
+      <c r="H94" t="s">
         <v>24</v>
       </c>
-      <c r="I94" s="2">
+      <c r="I94" s="7">
         <v>178567055</v>
       </c>
-      <c r="J94" s="4">
+      <c r="J94" s="5">
         <v>2605.98</v>
       </c>
       <c r="K94" s="2">
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row r="95" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>45468</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="7">
         <v>19045116278</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" t="s">
         <v>37</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" t="s">
         <v>21</v>
       </c>
-      <c r="E95" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F95" s="3" t="s">
+      <c r="E95" t="s">
+        <v>18</v>
+      </c>
+      <c r="F95" t="s">
         <v>14</v>
       </c>
       <c r="G95" s="1">
         <v>24352</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="H95" t="s">
         <v>24</v>
       </c>
-      <c r="I95" s="2">
+      <c r="I95" s="7">
         <v>762823951</v>
       </c>
-      <c r="J95" s="4">
+      <c r="J95" s="5">
         <v>1499.31</v>
       </c>
       <c r="K95" s="2">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row r="96" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>45468</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="7">
         <v>33755869063</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" t="s">
         <v>39</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" t="s">
         <v>21</v>
       </c>
-      <c r="E96" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="3" t="s">
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" t="s">
         <v>19</v>
       </c>
       <c r="G96" s="1">
         <v>38056</v>
       </c>
-      <c r="H96" s="3" t="s">
+      <c r="H96" t="s">
         <v>15</v>
       </c>
-      <c r="I96" s="2">
+      <c r="I96" s="7">
         <v>589868993</v>
       </c>
-      <c r="J96" s="4">
+      <c r="J96" s="5">
         <v>7067.54</v>
       </c>
       <c r="K96" s="2">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row r="97" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>45468</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="7">
         <v>80481414690</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" t="s">
         <v>37</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" t="s">
         <v>21</v>
       </c>
-      <c r="E97" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F97" s="3" t="s">
+      <c r="E97" t="s">
+        <v>18</v>
+      </c>
+      <c r="F97" t="s">
         <v>32</v>
       </c>
       <c r="G97" s="1">
         <v>32947</v>
       </c>
-      <c r="H97" s="3" t="s">
+      <c r="H97" t="s">
         <v>22</v>
       </c>
-      <c r="I97" s="2">
+      <c r="I97" s="7">
         <v>831728465</v>
       </c>
-      <c r="J97" s="4">
+      <c r="J97" s="5">
         <v>6978.76</v>
       </c>
       <c r="K97" s="2">
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row r="98" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>45468</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="7">
         <v>67427092600</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F98" s="3" t="s">
+      <c r="E98" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" t="s">
         <v>32</v>
       </c>
       <c r="G98" s="1">
         <v>29438</v>
       </c>
-      <c r="H98" s="3" t="s">
+      <c r="H98" t="s">
         <v>24</v>
       </c>
-      <c r="I98" s="2">
+      <c r="I98" s="7">
         <v>249593368</v>
       </c>
-      <c r="J98" s="4">
-        <v>8639.04</v>
+      <c r="J98" s="5">
+        <v>8639.0400000000009</v>
       </c>
       <c r="K98" s="2">
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row r="99" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>45468</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="7">
         <v>9376647076</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" t="s">
         <v>33</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" t="s">
         <v>21</v>
       </c>
-      <c r="E99" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F99" s="3" t="s">
+      <c r="E99" t="s">
+        <v>18</v>
+      </c>
+      <c r="F99" t="s">
         <v>14</v>
       </c>
       <c r="G99" s="1">
         <v>27201</v>
       </c>
-      <c r="H99" s="3" t="s">
+      <c r="H99" t="s">
         <v>24</v>
       </c>
-      <c r="I99" s="2">
+      <c r="I99" s="7">
         <v>824231340</v>
       </c>
-      <c r="J99" s="4">
-        <v>8635.7</v>
+      <c r="J99" s="5">
+        <v>8635.7000000000007</v>
       </c>
       <c r="K99" s="2">
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row r="100" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>45468</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="7">
         <v>15116071227</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" t="s">
         <v>21</v>
       </c>
-      <c r="E100" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="3" t="s">
+      <c r="E100" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" t="s">
         <v>14</v>
       </c>
       <c r="G100" s="1">
         <v>35457</v>
       </c>
-      <c r="H100" s="3" t="s">
+      <c r="H100" t="s">
         <v>24</v>
       </c>
-      <c r="I100" s="2">
+      <c r="I100" s="7">
         <v>194139312</v>
       </c>
-      <c r="J100" s="4">
+      <c r="J100" s="5">
         <v>6116.92</v>
       </c>
       <c r="K100" s="2">

</xml_diff>